<commit_message>
Parametrização de pesos de carga, spread e pico máximo de turmas permitido
</commit_message>
<xml_diff>
--- a/2_consolidado_instrutor_projeto.xlsx
+++ b/2_consolidado_instrutor_projeto.xlsx
@@ -495,25 +495,25 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>14</v>
@@ -526,22 +526,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>4</v>
@@ -560,28 +560,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
         <v>14</v>
@@ -597,10 +597,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
@@ -609,16 +609,16 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -634,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>3</v>
@@ -643,13 +643,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>14</v>
@@ -665,25 +665,25 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
         <v>14</v>
@@ -696,13 +696,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -714,13 +714,13 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -736,25 +736,25 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>3</v>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
@@ -779,13 +779,13 @@
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
         <v>14</v>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>3</v>
@@ -813,16 +813,16 @@
         <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -832,22 +832,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
         <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -869,28 +869,28 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -900,19 +900,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
         <v>2</v>
@@ -921,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -937,28 +937,28 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -971,19 +971,19 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="n">
         <v>2</v>
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -1005,28 +1005,28 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J17" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -1039,28 +1039,28 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -1073,10 +1073,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
         <v>2</v>
@@ -1085,13 +1085,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" t="n">
         <v>11</v>

</xml_diff>